<commit_message>
oopc, oopk, oopr - Aktualizacja wzorów statystyk miesięcznych aoppe, aopk, aopc2, aopc, aopk2, aopg, aopp - Aktualizacja wzorów statystyk miesięcznych
</commit_message>
<xml_diff>
--- a/Statystyki_2018/Template/aopk2.xlsx
+++ b/Statystyki_2018/Template/aopk2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t xml:space="preserve">lp</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t xml:space="preserve">skargi na przewlekłość</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uwagi</t>
   </si>
   <si>
     <r>
@@ -382,7 +385,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -508,13 +511,6 @@
     <font>
       <b val="true"/>
       <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
@@ -540,7 +536,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -560,6 +556,13 @@
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -620,6 +623,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -684,12 +691,8 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -709,15 +712,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:CA8"/>
+  <dimension ref="A3:CB7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BN1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CB3" activeCellId="0" sqref="CB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="0" width="30.31"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -822,6 +826,9 @@
       <c r="BY3" s="3"/>
       <c r="BZ3" s="3"/>
       <c r="CA3" s="3"/>
+      <c r="CB3" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
@@ -885,695 +892,464 @@
       <c r="BG4" s="4"/>
       <c r="BH4" s="4"/>
       <c r="BI4" s="4"/>
-      <c r="BJ4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="BK4" s="6"/>
-      <c r="BL4" s="6"/>
-      <c r="BM4" s="6"/>
-      <c r="BN4" s="6"/>
-      <c r="BO4" s="6"/>
-      <c r="BP4" s="6"/>
-      <c r="BQ4" s="6"/>
-      <c r="BR4" s="6"/>
-      <c r="BS4" s="6"/>
-      <c r="BT4" s="6"/>
-      <c r="BU4" s="6"/>
-      <c r="BV4" s="7" t="s">
+      <c r="BJ4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BW4" s="7"/>
+      <c r="BK4" s="7"/>
+      <c r="BL4" s="7"/>
+      <c r="BM4" s="7"/>
+      <c r="BN4" s="7"/>
+      <c r="BO4" s="7"/>
+      <c r="BP4" s="7"/>
+      <c r="BQ4" s="7"/>
+      <c r="BR4" s="7"/>
+      <c r="BS4" s="7"/>
+      <c r="BT4" s="7"/>
+      <c r="BU4" s="7"/>
+      <c r="BV4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="BW4" s="8"/>
       <c r="BX4" s="3"/>
       <c r="BY4" s="3"/>
       <c r="BZ4" s="3"/>
       <c r="CA4" s="3"/>
+      <c r="CB4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="24.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="F5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9" t="s">
+      <c r="I5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9" t="s">
+      <c r="J5" s="10"/>
+      <c r="K5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9" t="s">
+      <c r="M5" s="10"/>
+      <c r="N5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9" t="s">
+      <c r="O5" s="10"/>
+      <c r="P5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9" t="s">
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9" t="s">
+      <c r="S5" s="10"/>
+      <c r="T5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9" t="s">
+      <c r="U5" s="10"/>
+      <c r="V5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9" t="s">
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AP5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AE5" s="9" t="s">
+      <c r="AQ5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="AF5" s="9" t="s">
+      <c r="AR5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AG5" s="9" t="s">
+      <c r="AS5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AH5" s="9" t="s">
+      <c r="AT5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9" t="s">
+      <c r="AU5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AK5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL5" s="11" t="s">
+      <c r="AV5" s="10"/>
+      <c r="AW5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AM5" s="11"/>
-      <c r="AN5" s="11"/>
-      <c r="AO5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="AP5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AQ5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="AR5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="AT5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="AU5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="AV5" s="9"/>
-      <c r="AW5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="AX5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="AY5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="AZ5" s="13" t="s">
+      <c r="AY5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="BA5" s="13" t="s">
+      <c r="AZ5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="BB5" s="13" t="s">
+      <c r="BA5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="BC5" s="13" t="s">
+      <c r="BB5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="BD5" s="13" t="s">
+      <c r="BC5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="BE5" s="13" t="s">
+      <c r="BD5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="BF5" s="13" t="s">
+      <c r="BE5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="BG5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="BH5" s="14" t="s">
+      <c r="BF5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="BI5" s="14" t="s">
+      <c r="BG5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="BH5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="BJ5" s="13" t="s">
+      <c r="BI5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="BK5" s="15" t="s">
+      <c r="BJ5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="BL5" s="13" t="s">
+      <c r="BK5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="BM5" s="16" t="s">
+      <c r="BL5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="BN5" s="17" t="s">
+      <c r="BM5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="BO5" s="17"/>
-      <c r="BP5" s="17"/>
-      <c r="BQ5" s="17"/>
-      <c r="BR5" s="17"/>
-      <c r="BS5" s="17"/>
-      <c r="BT5" s="17"/>
-      <c r="BU5" s="17"/>
-      <c r="BV5" s="15" t="s">
+      <c r="BN5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="BW5" s="15"/>
-      <c r="BX5" s="18" t="s">
+      <c r="BO5" s="18"/>
+      <c r="BP5" s="18"/>
+      <c r="BQ5" s="18"/>
+      <c r="BR5" s="18"/>
+      <c r="BS5" s="18"/>
+      <c r="BT5" s="18"/>
+      <c r="BU5" s="18"/>
+      <c r="BV5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="BY5" s="19" t="s">
+      <c r="BW5" s="16"/>
+      <c r="BX5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="BZ5" s="19"/>
-      <c r="CA5" s="18" t="s">
+      <c r="BY5" s="20" t="s">
         <v>42</v>
       </c>
+      <c r="BZ5" s="20"/>
+      <c r="CA5" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="CB5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="14" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="20" t="s">
+      <c r="J6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="K6" s="10"/>
+      <c r="L6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="M6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="V6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="W6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="X6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="P6" s="20" t="s">
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="V6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="W6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="X6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI6" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ6" s="9"/>
-      <c r="AK6" s="10"/>
-      <c r="AL6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO6" s="12"/>
-      <c r="AP6" s="9"/>
-      <c r="AQ6" s="9"/>
-      <c r="AR6" s="9"/>
-      <c r="AS6" s="9"/>
-      <c r="AT6" s="9"/>
-      <c r="AU6" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV6" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW6" s="9"/>
-      <c r="AX6" s="10"/>
-      <c r="AY6" s="13"/>
-      <c r="AZ6" s="13"/>
-      <c r="BA6" s="13"/>
-      <c r="BB6" s="13"/>
-      <c r="BC6" s="13"/>
-      <c r="BD6" s="13"/>
-      <c r="BE6" s="13"/>
-      <c r="BF6" s="13"/>
-      <c r="BG6" s="14"/>
-      <c r="BH6" s="14"/>
-      <c r="BI6" s="14"/>
-      <c r="BJ6" s="13"/>
-      <c r="BK6" s="15"/>
-      <c r="BL6" s="13"/>
-      <c r="BM6" s="16"/>
-      <c r="BN6" s="17"/>
-      <c r="BO6" s="17"/>
-      <c r="BP6" s="17"/>
-      <c r="BQ6" s="17"/>
-      <c r="BR6" s="17"/>
-      <c r="BS6" s="17"/>
-      <c r="BT6" s="17"/>
-      <c r="BU6" s="17"/>
-      <c r="BV6" s="15"/>
-      <c r="BW6" s="15"/>
-      <c r="BX6" s="18"/>
-      <c r="BY6" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="BZ6" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="CA6" s="18"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="11"/>
+      <c r="AY6" s="14"/>
+      <c r="AZ6" s="14"/>
+      <c r="BA6" s="14"/>
+      <c r="BB6" s="14"/>
+      <c r="BC6" s="14"/>
+      <c r="BD6" s="14"/>
+      <c r="BE6" s="14"/>
+      <c r="BF6" s="14"/>
+      <c r="BG6" s="15"/>
+      <c r="BH6" s="15"/>
+      <c r="BI6" s="15"/>
+      <c r="BJ6" s="14"/>
+      <c r="BK6" s="16"/>
+      <c r="BL6" s="14"/>
+      <c r="BM6" s="17"/>
+      <c r="BN6" s="18"/>
+      <c r="BO6" s="18"/>
+      <c r="BP6" s="18"/>
+      <c r="BQ6" s="18"/>
+      <c r="BR6" s="18"/>
+      <c r="BS6" s="18"/>
+      <c r="BT6" s="18"/>
+      <c r="BU6" s="18"/>
+      <c r="BV6" s="16"/>
+      <c r="BW6" s="16"/>
+      <c r="BX6" s="19"/>
+      <c r="BY6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="BZ6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="CA6" s="19"/>
+      <c r="CB6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="105.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="111.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="20"/>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="8"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="14"/>
-      <c r="AI7" s="14"/>
-      <c r="AJ7" s="9"/>
-      <c r="AK7" s="10"/>
-      <c r="AL7" s="10"/>
-      <c r="AM7" s="10"/>
-      <c r="AN7" s="10"/>
-      <c r="AO7" s="12"/>
-      <c r="AP7" s="9"/>
-      <c r="AQ7" s="9"/>
-      <c r="AR7" s="9"/>
-      <c r="AS7" s="9"/>
-      <c r="AT7" s="9"/>
-      <c r="AU7" s="14"/>
-      <c r="AV7" s="14"/>
-      <c r="AW7" s="9"/>
-      <c r="AX7" s="10"/>
-      <c r="AY7" s="13"/>
-      <c r="AZ7" s="13"/>
-      <c r="BA7" s="13"/>
-      <c r="BB7" s="13"/>
-      <c r="BC7" s="13"/>
-      <c r="BD7" s="13"/>
-      <c r="BE7" s="13"/>
-      <c r="BF7" s="13"/>
-      <c r="BG7" s="14"/>
-      <c r="BH7" s="14"/>
-      <c r="BI7" s="14"/>
-      <c r="BJ7" s="13"/>
-      <c r="BK7" s="15"/>
-      <c r="BL7" s="13"/>
-      <c r="BM7" s="16"/>
-      <c r="BN7" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="BO7" s="18" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="15"/>
+      <c r="AI7" s="15"/>
+      <c r="AJ7" s="10"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11"/>
+      <c r="AM7" s="11"/>
+      <c r="AN7" s="11"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="10"/>
+      <c r="AQ7" s="10"/>
+      <c r="AR7" s="10"/>
+      <c r="AS7" s="10"/>
+      <c r="AT7" s="10"/>
+      <c r="AU7" s="15"/>
+      <c r="AV7" s="15"/>
+      <c r="AW7" s="10"/>
+      <c r="AX7" s="11"/>
+      <c r="AY7" s="14"/>
+      <c r="AZ7" s="14"/>
+      <c r="BA7" s="14"/>
+      <c r="BB7" s="14"/>
+      <c r="BC7" s="14"/>
+      <c r="BD7" s="14"/>
+      <c r="BE7" s="14"/>
+      <c r="BF7" s="14"/>
+      <c r="BG7" s="15"/>
+      <c r="BH7" s="15"/>
+      <c r="BI7" s="15"/>
+      <c r="BJ7" s="14"/>
+      <c r="BK7" s="16"/>
+      <c r="BL7" s="14"/>
+      <c r="BM7" s="17"/>
+      <c r="BN7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="BP7" s="18" t="s">
+      <c r="BO7" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="BQ7" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="BR7" s="18" t="s">
+      <c r="BP7" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="BS7" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="BT7" s="18" t="s">
+      <c r="BQ7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BR7" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="BU7" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="BV7" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="BW7" s="17" t="s">
+      <c r="BS7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BT7" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="BX7" s="18"/>
-      <c r="BY7" s="21"/>
-      <c r="BZ7" s="21"/>
-      <c r="CA7" s="18"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" s="23" t="n">
-        <v>4</v>
-      </c>
-      <c r="G8" s="23" t="n">
-        <v>5</v>
-      </c>
-      <c r="H8" s="23" t="n">
-        <v>6</v>
-      </c>
-      <c r="I8" s="23" t="n">
-        <v>7</v>
-      </c>
-      <c r="J8" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="K8" s="23" t="n">
-        <v>9</v>
-      </c>
-      <c r="L8" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="M8" s="23" t="n">
-        <v>11</v>
-      </c>
-      <c r="N8" s="23" t="n">
-        <v>12</v>
-      </c>
-      <c r="O8" s="23" t="n">
-        <v>13</v>
-      </c>
-      <c r="P8" s="23" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q8" s="23" t="n">
-        <v>15</v>
-      </c>
-      <c r="R8" s="23" t="n">
-        <v>16</v>
-      </c>
-      <c r="S8" s="23" t="n">
-        <v>17</v>
-      </c>
-      <c r="T8" s="23" t="n">
-        <v>18</v>
-      </c>
-      <c r="U8" s="23" t="n">
-        <v>19</v>
-      </c>
-      <c r="V8" s="23" t="n">
-        <v>20</v>
-      </c>
-      <c r="W8" s="23" t="n">
-        <v>21</v>
-      </c>
-      <c r="X8" s="23" t="n">
-        <v>22</v>
-      </c>
-      <c r="Y8" s="23" t="n">
+      <c r="BU7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BV7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="Z8" s="23" t="n">
-        <v>24</v>
-      </c>
-      <c r="AA8" s="23" t="n">
-        <v>25</v>
-      </c>
-      <c r="AB8" s="23" t="n">
-        <v>26</v>
-      </c>
-      <c r="AC8" s="23" t="n">
-        <v>27</v>
-      </c>
-      <c r="AD8" s="23" t="n">
-        <v>28</v>
-      </c>
-      <c r="AE8" s="23" t="n">
-        <v>29</v>
-      </c>
-      <c r="AF8" s="23" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG8" s="23" t="n">
-        <v>31</v>
-      </c>
-      <c r="AH8" s="23" t="n">
-        <v>32</v>
-      </c>
-      <c r="AI8" s="23" t="n">
-        <v>33</v>
-      </c>
-      <c r="AJ8" s="23" t="n">
-        <v>34</v>
-      </c>
-      <c r="AK8" s="23" t="n">
-        <v>35</v>
-      </c>
-      <c r="AL8" s="23" t="n">
-        <v>36</v>
-      </c>
-      <c r="AM8" s="23" t="n">
-        <v>37</v>
-      </c>
-      <c r="AN8" s="23" t="n">
-        <v>38</v>
-      </c>
-      <c r="AO8" s="23" t="n">
-        <v>39</v>
-      </c>
-      <c r="AP8" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="AQ8" s="23" t="n">
-        <v>41</v>
-      </c>
-      <c r="AR8" s="23" t="n">
-        <v>42</v>
-      </c>
-      <c r="AS8" s="23" t="n">
-        <v>43</v>
-      </c>
-      <c r="AT8" s="23" t="n">
-        <v>44</v>
-      </c>
-      <c r="AU8" s="23" t="n">
-        <v>45</v>
-      </c>
-      <c r="AV8" s="23" t="n">
-        <v>46</v>
-      </c>
-      <c r="AW8" s="23" t="n">
-        <v>47</v>
-      </c>
-      <c r="AX8" s="23" t="n">
-        <v>48</v>
-      </c>
-      <c r="AY8" s="23" t="n">
-        <v>49</v>
-      </c>
-      <c r="AZ8" s="23" t="n">
-        <v>50</v>
-      </c>
-      <c r="BA8" s="23" t="n">
-        <v>51</v>
-      </c>
-      <c r="BB8" s="23" t="n">
-        <v>52</v>
-      </c>
-      <c r="BC8" s="23" t="n">
-        <v>53</v>
-      </c>
-      <c r="BD8" s="23" t="n">
-        <v>54</v>
-      </c>
-      <c r="BE8" s="23" t="n">
-        <v>55</v>
-      </c>
-      <c r="BF8" s="23" t="n">
-        <v>56</v>
-      </c>
-      <c r="BG8" s="23" t="n">
+      <c r="BW7" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="BH8" s="23" t="n">
-        <v>58</v>
-      </c>
-      <c r="BI8" s="23" t="n">
-        <v>59</v>
-      </c>
-      <c r="BJ8" s="23" t="n">
-        <v>60</v>
-      </c>
-      <c r="BK8" s="23" t="n">
-        <v>61</v>
-      </c>
-      <c r="BL8" s="23" t="n">
-        <v>62</v>
-      </c>
-      <c r="BM8" s="23" t="n">
-        <v>63</v>
-      </c>
-      <c r="BN8" s="23" t="n">
-        <v>64</v>
-      </c>
-      <c r="BO8" s="23" t="n">
-        <v>65</v>
-      </c>
-      <c r="BP8" s="23" t="n">
-        <v>66</v>
-      </c>
-      <c r="BQ8" s="23" t="n">
-        <v>67</v>
-      </c>
-      <c r="BR8" s="23" t="n">
-        <v>68</v>
-      </c>
-      <c r="BS8" s="23" t="n">
-        <v>69</v>
-      </c>
-      <c r="BT8" s="23" t="n">
-        <v>70</v>
-      </c>
-      <c r="BU8" s="23" t="n">
-        <v>71</v>
-      </c>
-      <c r="BV8" s="23" t="n">
-        <v>72</v>
-      </c>
-      <c r="BW8" s="23" t="n">
-        <v>73</v>
-      </c>
-      <c r="BX8" s="23" t="n">
-        <v>74</v>
-      </c>
-      <c r="BY8" s="23" t="n">
-        <v>75</v>
-      </c>
-      <c r="BZ8" s="23" t="n">
-        <v>76</v>
-      </c>
-      <c r="CA8" s="23" t="n">
-        <v>77</v>
-      </c>
+      <c r="BX7" s="19"/>
+      <c r="BY7" s="22"/>
+      <c r="BZ7" s="22"/>
+      <c r="CA7" s="19"/>
+      <c r="CB7" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="95">
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="B3:B8"/>
+  <mergeCells count="96">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
     <mergeCell ref="C3:K4"/>
     <mergeCell ref="L3:AA4"/>
     <mergeCell ref="AB3:AJ4"/>
@@ -1583,6 +1359,7 @@
     <mergeCell ref="BG3:BI4"/>
     <mergeCell ref="BJ3:BW3"/>
     <mergeCell ref="BX3:CA4"/>
+    <mergeCell ref="CB3:CB7"/>
     <mergeCell ref="BJ4:BU4"/>
     <mergeCell ref="BV4:BW4"/>
     <mergeCell ref="C5:C7"/>

</xml_diff>